<commit_message>
updated sangao template file.
</commit_message>
<xml_diff>
--- a/xbrx_12345_excel_tool/templates/sangao_template.xlsx
+++ b/xbrx_12345_excel_tool/templates/sangao_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22440" windowHeight="11790"/>
+    <workbookView windowWidth="22440" windowHeight="11790" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -204,225 +204,225 @@
     <t>表井维修</t>
   </si>
   <si>
+    <t>普利市政管网公司</t>
+  </si>
+  <si>
+    <t>方形井盖补换</t>
+  </si>
+  <si>
+    <t>东区供水公司</t>
+  </si>
+  <si>
+    <t>换表后漏水</t>
+  </si>
+  <si>
+    <t>营业部</t>
+  </si>
+  <si>
+    <t>换表维修后无水</t>
+  </si>
+  <si>
+    <t>二次供水管理部</t>
+  </si>
+  <si>
+    <t>水表自转</t>
+  </si>
+  <si>
+    <t>客户发展部</t>
+  </si>
+  <si>
+    <t>表蒙子漏水</t>
+  </si>
+  <si>
+    <t>水质中心</t>
+  </si>
+  <si>
+    <t>水表丢失</t>
+  </si>
+  <si>
+    <t>工程管理部</t>
+  </si>
+  <si>
+    <t>水表损坏</t>
+  </si>
+  <si>
+    <t>普润水务</t>
+  </si>
+  <si>
+    <t>水表更换</t>
+  </si>
+  <si>
+    <t>加压供水管理部</t>
+  </si>
+  <si>
+    <t>水量的异议</t>
+  </si>
+  <si>
+    <t>房地产物业管理部</t>
+  </si>
+  <si>
+    <t>表止度的异议</t>
+  </si>
+  <si>
+    <t>稽查大队</t>
+  </si>
+  <si>
+    <t>违约金的异议</t>
+  </si>
+  <si>
+    <t>安全生产部</t>
+  </si>
+  <si>
+    <t>抄收服务</t>
+  </si>
+  <si>
+    <t>长清供水公司</t>
+  </si>
+  <si>
+    <t>退费核减</t>
+  </si>
+  <si>
+    <t>西城供水公司</t>
+  </si>
+  <si>
+    <t>对各类通知单及短信的异议</t>
+  </si>
+  <si>
+    <t>南山供水</t>
+  </si>
+  <si>
+    <t>处理方案未落实</t>
+  </si>
+  <si>
+    <t>普利工程公司</t>
+  </si>
+  <si>
+    <t>井室整治</t>
+  </si>
+  <si>
+    <t>热线科</t>
+  </si>
+  <si>
+    <t>井盖补换</t>
+  </si>
+  <si>
     <t>设施科</t>
   </si>
   <si>
-    <t>方形井盖补换</t>
-  </si>
-  <si>
-    <t>稽查大队</t>
-  </si>
-  <si>
-    <t>换表后漏水</t>
+    <t>表箱改造整治</t>
+  </si>
+  <si>
+    <t>管网部</t>
+  </si>
+  <si>
+    <t>内部协调</t>
+  </si>
+  <si>
+    <t>泓泉制水公司</t>
+  </si>
+  <si>
+    <t>闸门开关</t>
+  </si>
+  <si>
+    <t>泉娃饮用水公司</t>
+  </si>
+  <si>
+    <t>闸门开关DN&lt;300</t>
+  </si>
+  <si>
+    <t>信息中心</t>
+  </si>
+  <si>
+    <t>闸门开关DN≥300</t>
+  </si>
+  <si>
+    <t>人力资源部</t>
+  </si>
+  <si>
+    <t>转派其他部门</t>
+  </si>
+  <si>
+    <t>服务督查科</t>
+  </si>
+  <si>
+    <t>区域性无水水压低</t>
+  </si>
+  <si>
+    <t>管网工程公司</t>
+  </si>
+  <si>
+    <t>单户无水水压低</t>
+  </si>
+  <si>
+    <t>普天检漏公司</t>
+  </si>
+  <si>
+    <t>二供设备无水水压低</t>
+  </si>
+  <si>
+    <t>企业管理部</t>
+  </si>
+  <si>
+    <t>管道损坏漏水</t>
+  </si>
+  <si>
+    <t>保卫部</t>
+  </si>
+  <si>
+    <t>闸门损坏漏水</t>
+  </si>
+  <si>
+    <t>总工办</t>
+  </si>
+  <si>
+    <t>消防损坏漏水</t>
+  </si>
+  <si>
+    <t>财务部</t>
+  </si>
+  <si>
+    <t>闸门井盖损坏</t>
   </si>
   <si>
     <t>水厂项目部</t>
   </si>
   <si>
-    <t>换表维修后无水</t>
-  </si>
-  <si>
-    <t>人力资源部</t>
-  </si>
-  <si>
-    <t>水表自转</t>
-  </si>
-  <si>
-    <t>泉娃饮用水公司</t>
-  </si>
-  <si>
-    <t>表蒙子漏水</t>
-  </si>
-  <si>
-    <t>房地产物业管理部</t>
-  </si>
-  <si>
-    <t>水表丢失</t>
-  </si>
-  <si>
-    <t>普润水务</t>
-  </si>
-  <si>
-    <t>水表损坏</t>
-  </si>
-  <si>
-    <t>客户发展部</t>
-  </si>
-  <si>
-    <t>水表更换</t>
+    <t>管廊漏水</t>
+  </si>
+  <si>
+    <t>设计院</t>
+  </si>
+  <si>
+    <t>局部管线更换</t>
   </si>
   <si>
     <t>客服中心</t>
   </si>
   <si>
-    <t>水量的异议</t>
-  </si>
-  <si>
-    <t>普利工程公司</t>
-  </si>
-  <si>
-    <t>表止度的异议</t>
-  </si>
-  <si>
-    <t>南山供水</t>
-  </si>
-  <si>
-    <t>违约金的异议</t>
-  </si>
-  <si>
-    <t>安全生产部</t>
-  </si>
-  <si>
-    <t>抄收服务</t>
-  </si>
-  <si>
-    <t>设计院</t>
-  </si>
-  <si>
-    <t>退费核减</t>
-  </si>
-  <si>
-    <t>工程管理部</t>
-  </si>
-  <si>
-    <t>对各类通知单及短信的异议</t>
-  </si>
-  <si>
-    <t>水质中心</t>
-  </si>
-  <si>
-    <t>处理方案未落实</t>
-  </si>
-  <si>
-    <t>泓泉制水公司</t>
-  </si>
-  <si>
-    <t>井室整治</t>
+    <t>废旧管线掐管</t>
   </si>
   <si>
     <t>办公室</t>
   </si>
   <si>
-    <t>井盖补换</t>
-  </si>
-  <si>
-    <t>西城供水公司</t>
-  </si>
-  <si>
-    <t>表箱改造整治</t>
-  </si>
-  <si>
-    <t>企业管理部</t>
-  </si>
-  <si>
-    <t>内部协调</t>
-  </si>
-  <si>
-    <t>加压供水管理部</t>
-  </si>
-  <si>
-    <t>闸门开关</t>
-  </si>
-  <si>
-    <t>信息中心</t>
-  </si>
-  <si>
-    <t>闸门开关DN&lt;300</t>
-  </si>
-  <si>
-    <t>营业部</t>
-  </si>
-  <si>
-    <t>闸门开关DN≥300</t>
-  </si>
-  <si>
-    <t>管网部</t>
-  </si>
-  <si>
-    <t>转派其他部门</t>
-  </si>
-  <si>
-    <t>管网工程公司</t>
-  </si>
-  <si>
-    <t>区域性无水水压低</t>
-  </si>
-  <si>
-    <t>东区供水公司</t>
-  </si>
-  <si>
-    <t>单户无水水压低</t>
-  </si>
-  <si>
-    <t>保卫部</t>
-  </si>
-  <si>
-    <t>二供设备无水水压低</t>
-  </si>
-  <si>
-    <t>普利市政管网公司</t>
-  </si>
-  <si>
-    <t>管道损坏漏水</t>
-  </si>
-  <si>
-    <t>财务部</t>
-  </si>
-  <si>
-    <t>闸门损坏漏水</t>
+    <t>闸门丼室整治</t>
   </si>
   <si>
     <t>生技科</t>
   </si>
   <si>
-    <t>消防损坏漏水</t>
-  </si>
-  <si>
-    <t>总工办</t>
-  </si>
-  <si>
-    <t>闸门井盖损坏</t>
-  </si>
-  <si>
-    <t>服务督查科</t>
-  </si>
-  <si>
-    <t>管廊漏水</t>
+    <t>闸门故障</t>
   </si>
   <si>
     <t>检漏科</t>
   </si>
   <si>
-    <t>局部管线更换</t>
-  </si>
-  <si>
-    <t>普天检漏公司</t>
-  </si>
-  <si>
-    <t>废旧管线掐管</t>
-  </si>
-  <si>
-    <t>长清供水公司</t>
-  </si>
-  <si>
-    <t>闸门丼室整治</t>
-  </si>
-  <si>
-    <t>二次供水管理部</t>
-  </si>
-  <si>
-    <t>闸门故障</t>
+    <t>消防维护</t>
   </si>
   <si>
     <t>管网所</t>
   </si>
   <si>
-    <t>消防维护</t>
-  </si>
-  <si>
-    <t>热线科</t>
-  </si>
-  <si>
     <t>施工回填</t>
   </si>
   <si>
@@ -567,7 +567,7 @@
     <t>施工扰民无围挡</t>
   </si>
   <si>
-    <t>施工扰民其他扰民</t>
+    <t>其他施工扰民</t>
   </si>
   <si>
     <t xml:space="preserve">直饮水无水 </t>
@@ -654,8 +654,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -693,6 +693,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -700,14 +707,61 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -723,37 +777,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -766,22 +790,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -789,7 +807,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -804,37 +822,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -851,187 +851,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,6 +1060,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1071,17 +1095,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1103,9 +1116,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1127,36 +1157,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1165,10 +1165,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1177,133 +1177,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1645,7 +1645,7 @@
   <sheetPr/>
   <dimension ref="A1:AW1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1809,12 +1809,12 @@
     </row>
   </sheetData>
   <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576 C$1:C$1048576 D$1:D$1048576 E$1:E$1048576">
+      <formula1>Sheet2!$B$2:$B$23</formula1>
+    </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 F717:F1048576"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
       <formula1>Sheet2!$A$2:$A$118</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576 C$1:C$1048576 D$1:D$1048576 E$1:E$1048576">
-      <formula1>Sheet2!$B$2:$B$43</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F716">
       <formula1>"是,否"</formula1>
@@ -1831,8 +1831,8 @@
   <sheetPr/>
   <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>

</xml_diff>